<commit_message>
Avec plans inserts. Reedom : images déjà compressé
</commit_message>
<xml_diff>
--- a/SU - Suspension/Cost/cost_SU_A0100.xlsx
+++ b/SU - Suspension/Cost/cost_SU_A0100.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <fileSharing readOnlyRecommended="1"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julien Lazure\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphaël\Desktop\ECL\2A\EPSA\Cost_Report_Vulcanix\Cost_SU\Cost_Julien\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD185840-4685-4626-85E8-2EBF74C98F41}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4740" yWindow="60" windowWidth="16380" windowHeight="8190" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -164,7 +165,7 @@
     <definedName name="zer">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">BOM!$A$1:$N$18</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -892,7 +893,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="16">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(\$* #,##0.00_);_(\$* \(#,##0.00\);_(\$* \-??_);_(@_)"/>
@@ -1636,7 +1637,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -1937,40 +1938,41 @@
     <xf numFmtId="4" fontId="28" fillId="0" borderId="28" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="31" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="28" fillId="0" borderId="28" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="32">
-    <cellStyle name="Comma 2" xfId="5"/>
-    <cellStyle name="Cost Table Plain" xfId="10"/>
-    <cellStyle name="Cost_Green" xfId="4"/>
-    <cellStyle name="Cost_Yellow" xfId="11"/>
-    <cellStyle name="Currency 2" xfId="2"/>
-    <cellStyle name="Currency 2 2" xfId="12"/>
-    <cellStyle name="Good 2" xfId="13"/>
+    <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Cost Table Plain" xfId="10" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Cost_Green" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Cost_Yellow" xfId="11" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Currency 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Currency 2 2" xfId="12" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Good 2" xfId="13" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Lien hypertexte" xfId="8" builtinId="8"/>
-    <cellStyle name="Monétaire 10 2" xfId="29"/>
-    <cellStyle name="Monétaire 2" xfId="3"/>
-    <cellStyle name="Monétaire 3" xfId="14"/>
+    <cellStyle name="Monétaire 10 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Monétaire 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Monétaire 3" xfId="14" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="15"/>
-    <cellStyle name="Normal 2 2 2" xfId="16"/>
-    <cellStyle name="Normal 2 2 2 2" xfId="17"/>
-    <cellStyle name="Normal 2 2 2 2 2" xfId="18"/>
-    <cellStyle name="Normal 2 2 2 3" xfId="19"/>
-    <cellStyle name="Normal 2 2 3" xfId="20"/>
-    <cellStyle name="Normal 2 2 4" xfId="21"/>
-    <cellStyle name="Normal 2 2 4 2" xfId="22"/>
-    <cellStyle name="Normal 2 3" xfId="23"/>
-    <cellStyle name="Normal 2 4" xfId="24"/>
-    <cellStyle name="Normal 3" xfId="6"/>
-    <cellStyle name="Normal 3 2" xfId="26"/>
-    <cellStyle name="Normal 3 3" xfId="25"/>
-    <cellStyle name="Normal 3 4" xfId="31"/>
-    <cellStyle name="Normal 4" xfId="9"/>
-    <cellStyle name="Normal 5" xfId="27"/>
-    <cellStyle name="Normal_Sheet1" xfId="30"/>
-    <cellStyle name="Style 1" xfId="28"/>
-    <cellStyle name="TableStyleLight1" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 2 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 2 2 2 2" xfId="17" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 2 2 2 2 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 2 2 2 3" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal 2 2 3" xfId="20" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal 2 2 4" xfId="21" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal 2 2 4 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal 2 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal 2 4" xfId="24" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Normal 3 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Normal 3 3" xfId="25" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Normal 3 4" xfId="31" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="Normal 4" xfId="9" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 5" xfId="27" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Normal_Sheet1" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="Style 1" xfId="28" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="TableStyleLight1" xfId="7" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2078,7 +2080,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2114,20 +2122,136 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>426640</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>704452</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>59532</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>168672</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>556550</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>370283</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>166289</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>92471</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6538516" y="2619375"/>
+          <a:ext cx="3192461" cy="2394346"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>626969</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>49306</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>17369</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>165287</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8941734" y="2335306"/>
+          <a:ext cx="3200400" cy="2401981"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>644169</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>101630</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{368D1A18-0015-46D2-8028-9BDAF137451A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2146,8 +2270,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7570390" y="3343671"/>
-          <a:ext cx="3364441" cy="2523331"/>
+          <a:off x="47625" y="266700"/>
+          <a:ext cx="8387994" cy="5930930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2156,106 +2280,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9553575" y="2733675"/>
-          <a:ext cx="3200400" cy="2400300"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="6019903" cy="2863928"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="dEL_010001">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="352425" y="533400"/>
-          <a:ext cx="6019903" cy="2863928"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2273,6 +2297,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Image 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -2319,6 +2348,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Image 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -2365,6 +2399,11 @@
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="Image 1">
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
@@ -2553,6 +2592,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2588,6 +2644,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2763,7 +2836,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -3114,15 +3187,15 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF66"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3141,7 +3214,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" location="SU_01001!B5" display="SU_01001!B5"/>
+    <hyperlink ref="B1" location="SU_01001!B5" display="SU_01001!B5" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -3150,14 +3223,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3178,7 +3251,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" location="SU_01002!B5" display="SU_01002!B5"/>
+    <hyperlink ref="B1" location="SU_01002!B5" display="SU_01002!B5" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3186,7 +3259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -3211,7 +3284,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" location="SU_01005!B5" display="SU_01005"/>
+    <hyperlink ref="B1" location="SU_01005!B5" display="SU_01005" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3219,7 +3292,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -3250,8 +3323,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" location="SU_01006!B5" display="SU_01006"/>
-    <hyperlink ref="L58" location="BR_01001" display="BR_01001"/>
+    <hyperlink ref="B1" location="SU_01006!B5" display="SU_01006" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="L58" location="BR_01001" display="BR_01001" xr:uid="{00000000-0004-0000-0C00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3259,7 +3332,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6004,8 +6077,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F7" location="BR_A0001" display="BR_A0001"/>
-    <hyperlink ref="F8" location="BR_01001" display="BR_01001"/>
+    <hyperlink ref="F7" location="BR_A0001" display="BR_A0001" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F8" location="BR_01001" display="BR_01001" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.41" right="0.22" top="0.72" bottom="0.57999999999999996" header="0.5" footer="0.26"/>
   <pageSetup scale="61" fitToHeight="99" orientation="landscape" r:id="rId1"/>
@@ -6017,7 +6090,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
     <pageSetUpPr fitToPage="1"/>
@@ -7547,13 +7620,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" location="BR_01001" display="BR_01001"/>
-    <hyperlink ref="B11:B13" location="BR_01001" display="BR_01001"/>
-    <hyperlink ref="B14" location="SU_01005!B5" display="SU_01005!B5"/>
-    <hyperlink ref="B15" location="SU_01006!B5" display="SU_01006!B5"/>
-    <hyperlink ref="B11" location="SU_01002!B5" display="SU_01002!B5"/>
-    <hyperlink ref="B12" location="SU_01003!B5" display="SU_01003!B5"/>
-    <hyperlink ref="B13" location="SU_01004!B5" display="SU_01004!B5"/>
+    <hyperlink ref="B10" location="BR_01001" display="BR_01001" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B11:B13" location="BR_01001" display="BR_01001" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B14" location="SU_01005!B5" display="SU_01005!B5" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B15" location="SU_01006!B5" display="SU_01006!B5" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B11" location="SU_01002!B5" display="SU_01002!B5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B12" location="SU_01003!B5" display="SU_01003!B5" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B13" location="SU_01004!B5" display="SU_01004!B5" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup paperSize="9" scale="39" firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -7568,7 +7641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF66"/>
     <pageSetUpPr fitToPage="1"/>
@@ -7576,7 +7649,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7868,7 +7941,7 @@
       <c r="I11" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="J11" s="106">
+      <c r="J11" s="177">
         <f>90*90</f>
         <v>8100</v>
       </c>
@@ -8200,8 +8273,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001"/>
-    <hyperlink ref="E3" location="dBR_01001" display="Drawing"/>
+    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E3" location="dBR_01001" display="Drawing" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" scale="43" firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -8218,14 +8291,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF66"/>
   </sheetPr>
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8865,8 +8938,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001"/>
-    <hyperlink ref="E3" location="dBR_01001" display="Drawing"/>
+    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="E3" location="dBR_01001" display="Drawing" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8874,13 +8947,13 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF66"/>
   </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -9340,20 +9413,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001"/>
+    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF66"/>
   </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -9813,15 +9886,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001"/>
-    <hyperlink ref="E3" location="dBR_01001" display="Drawing"/>
+    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="E3" location="dBR_01001" display="Drawing" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF66"/>
   </sheetPr>
@@ -10451,21 +10524,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001"/>
-    <hyperlink ref="E3" location="'SU Drawing Part 5'!A1" display="Drawing"/>
+    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="E3" location="'SU Drawing Part 5'!A1" display="Drawing" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFFF66"/>
   </sheetPr>
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -11026,8 +11099,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001"/>
-    <hyperlink ref="E3" location="'SU Drawing Part 6'!A1" display="Drawing"/>
+    <hyperlink ref="B4" location="BR_A0001" display="BR_A0001" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="E3" location="'SU Drawing Part 6'!A1" display="Drawing" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
COST Su de mes couilles
</commit_message>
<xml_diff>
--- a/SU - Suspension/Cost/cost_SU_A0100.xlsx
+++ b/SU - Suspension/Cost/cost_SU_A0100.xlsx
@@ -10,7 +10,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7548" firstSheet="3" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="7" r:id="rId1"/>
@@ -29,12 +29,18 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <definedNames>
     <definedName name="dSU_01001">'dSU 01001'!$A$1</definedName>
     <definedName name="dSU_01002">'dSU 01002'!$A$1</definedName>
     <definedName name="dSU_01005">'dSU 01005'!$A$1</definedName>
     <definedName name="dSU_01006">'dSU 01006'!$A$1</definedName>
+    <definedName name="FR_01001_q">'[2]FR 01001'!$N$3</definedName>
+    <definedName name="FR_01002_q">'[2]FR 01002'!$N$3</definedName>
+    <definedName name="FR_01003_q">'[2]FR 01003'!$N$3</definedName>
+    <definedName name="FR_01004_q">'[2]FR 01004'!$N$3</definedName>
+    <definedName name="FR_A0001_q">'[2]FR A0100'!$N$3</definedName>
     <definedName name="SU_01001">'SU 01001'!$B$6</definedName>
     <definedName name="SU_01001_m">'SU 01001'!$N$12</definedName>
     <definedName name="SU_01001_p">'SU 01001'!$I$21</definedName>
@@ -60,6 +66,7 @@
     <definedName name="SU_01006_p">'SU 01006'!$I$19</definedName>
     <definedName name="SU_01006_q">'SU 01006'!$N$3</definedName>
     <definedName name="SU_A0100">'SU A0100'!$B$5</definedName>
+    <definedName name="SU_A0100_BOM">BOM!$C$7</definedName>
     <definedName name="SU_A0100_f">'SU A0100'!$J$50</definedName>
     <definedName name="SU_A0100_m">'SU A0100'!$N$22</definedName>
     <definedName name="SU_A0100_p">'SU A0100'!$I$43</definedName>
@@ -1538,7 +1545,7 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="178">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="13" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
@@ -1732,14 +1739,7 @@
     <xf numFmtId="18" fontId="13" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="172" fontId="13" fillId="9" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="37" fontId="13" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="172" fontId="13" fillId="9" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1759,20 +1759,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="18" fontId="13" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="18" fontId="13" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="3" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="172" fontId="13" fillId="10" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="37" fontId="13" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="172" fontId="13" fillId="10" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1801,7 +1793,6 @@
     <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="7">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="9"/>
     <xf numFmtId="165" fontId="28" fillId="0" borderId="29" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="165" fontId="28" fillId="0" borderId="3" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="39" fontId="28" fillId="0" borderId="28" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1840,6 +1831,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="28" xfId="31" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="28" fillId="0" borderId="28" xfId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="18" fontId="20" fillId="9" borderId="3" xfId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="32">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -2287,6 +2281,54 @@
 
 <file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>242723</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="15216" t="9023" r="10549"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10145485" y="2318657"/>
+          <a:ext cx="1940895" cy="1458686"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -2358,11 +2400,6 @@
             <v>Suspension &amp; Shocks</v>
           </cell>
         </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>Lower Front A-arm</v>
-          </cell>
-        </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="5">
@@ -2380,6 +2417,211 @@
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="BOM"/>
+      <sheetName val="FR A0100"/>
+      <sheetName val="FR 01001"/>
+      <sheetName val="FR 01002"/>
+      <sheetName val="FR 01003"/>
+      <sheetName val="FR 01004"/>
+      <sheetName val="dFR 01004"/>
+      <sheetName val="FR A0200"/>
+      <sheetName val="FR 02001"/>
+      <sheetName val="FR A0300"/>
+      <sheetName val="FR_03001"/>
+      <sheetName val="dFR_03001"/>
+      <sheetName val="FR_03002"/>
+      <sheetName val="dFR_03002"/>
+      <sheetName val="FR_03003"/>
+      <sheetName val="dFR_03003"/>
+      <sheetName val="FR_03004"/>
+      <sheetName val="dFR_03004"/>
+      <sheetName val="FR_03005"/>
+      <sheetName val="dFR_03005"/>
+      <sheetName val="FR_03006"/>
+      <sheetName val="dFR_03006"/>
+      <sheetName val="FR_03007"/>
+      <sheetName val="dFR_03007"/>
+      <sheetName val="FR_03008"/>
+      <sheetName val="dFR_03008"/>
+      <sheetName val="FR_03009"/>
+      <sheetName val="dFR_03009"/>
+      <sheetName val="FR_03010"/>
+      <sheetName val="dFR_03010"/>
+      <sheetName val="FR_03011"/>
+      <sheetName val="dFR_03011"/>
+      <sheetName val="FR_03012"/>
+      <sheetName val="dFR_03012"/>
+      <sheetName val="FR_03013"/>
+      <sheetName val="dFR_03013"/>
+      <sheetName val="FR_03014"/>
+      <sheetName val="dFR_03014"/>
+      <sheetName val="FR A0400"/>
+      <sheetName val="FR_04001"/>
+      <sheetName val="dFR_04001"/>
+      <sheetName val="FR_04002"/>
+      <sheetName val="dFR_04002"/>
+      <sheetName val="FR_04003"/>
+      <sheetName val="dFR_04003"/>
+      <sheetName val="FR A0500"/>
+      <sheetName val="FR 05001"/>
+      <sheetName val="dFR 05001"/>
+      <sheetName val="FR 05002"/>
+      <sheetName val="FR 05003"/>
+      <sheetName val="FR 05004"/>
+      <sheetName val="FR 05005"/>
+      <sheetName val="FR A0600"/>
+      <sheetName val="FR 06001"/>
+      <sheetName val="FR 06002"/>
+      <sheetName val="FR 06003"/>
+      <sheetName val="FR 06004"/>
+      <sheetName val="dFR 06004"/>
+      <sheetName val="FR 06005"/>
+      <sheetName val="dFR 06005"/>
+      <sheetName val="FR 06006"/>
+      <sheetName val="FR A0700"/>
+      <sheetName val="FR_07001"/>
+      <sheetName val="dFR_07001"/>
+      <sheetName val="FR_07002"/>
+      <sheetName val="dFR_07002"/>
+      <sheetName val="FR_07003"/>
+      <sheetName val="dFR_07003"/>
+      <sheetName val="FR_07004"/>
+      <sheetName val="dFR_07004"/>
+      <sheetName val="FR_07005"/>
+      <sheetName val="dFR_07005"/>
+      <sheetName val="FR_07006"/>
+      <sheetName val="dFR_07006"/>
+      <sheetName val="FR_07007"/>
+      <sheetName val="dFR_07007"/>
+      <sheetName val="FR_07008"/>
+      <sheetName val="dFR_07008"/>
+      <sheetName val="FR A0800"/>
+      <sheetName val="FR 08001"/>
+      <sheetName val="FR 08002"/>
+      <sheetName val="FR 08003"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="N3">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="3">
+          <cell r="N3">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="3">
+          <cell r="N3">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="3">
+          <cell r="N3">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="3">
+          <cell r="N3">
+            <v>4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
+      <sheetData sheetId="68"/>
+      <sheetData sheetId="69"/>
+      <sheetData sheetId="70"/>
+      <sheetData sheetId="71"/>
+      <sheetData sheetId="72"/>
+      <sheetData sheetId="73"/>
+      <sheetData sheetId="74"/>
+      <sheetData sheetId="75"/>
+      <sheetData sheetId="76"/>
+      <sheetData sheetId="77"/>
+      <sheetData sheetId="78"/>
+      <sheetData sheetId="79"/>
+      <sheetData sheetId="80"/>
+      <sheetData sheetId="81"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3029,7 +3271,7 @@
   <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3068,7 +3310,7 @@
       <c r="D2" s="58"/>
       <c r="E2" s="58"/>
       <c r="F2" s="58"/>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="97" t="s">
         <v>127</v>
       </c>
       <c r="H2" s="58"/>
@@ -3313,7 +3555,7 @@
       <c r="D11" s="31">
         <v>2.25</v>
       </c>
-      <c r="E11" s="157">
+      <c r="E11" s="152">
         <f>J11*K11*L11/1000000000</f>
         <v>1.5775360000000002E-2</v>
       </c>
@@ -3343,7 +3585,7 @@
         <v>3.5494560000000008E-2</v>
       </c>
       <c r="O11" s="69"/>
-      <c r="Q11" s="155"/>
+      <c r="Q11" s="150"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="70"/>
@@ -3455,7 +3697,7 @@
       <c r="A16" s="66">
         <v>20</v>
       </c>
-      <c r="B16" s="154" t="s">
+      <c r="B16" s="149" t="s">
         <v>184</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -3467,7 +3709,7 @@
       <c r="E16" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="F16" s="160">
+      <c r="F16" s="155">
         <v>0.4</v>
       </c>
       <c r="G16" s="28"/>
@@ -3487,7 +3729,7 @@
       <c r="A17" s="94">
         <v>30</v>
       </c>
-      <c r="B17" s="154" t="s">
+      <c r="B17" s="149" t="s">
         <v>183</v>
       </c>
       <c r="C17" s="27" t="s">
@@ -3519,7 +3761,7 @@
       <c r="A18" s="66">
         <v>40</v>
       </c>
-      <c r="B18" s="154" t="s">
+      <c r="B18" s="149" t="s">
         <v>184</v>
       </c>
       <c r="C18" s="19" t="s">
@@ -3531,7 +3773,7 @@
       <c r="E18" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="F18" s="160">
+      <c r="F18" s="155">
         <v>0.56000000000000005</v>
       </c>
       <c r="G18" s="28"/>
@@ -3551,7 +3793,7 @@
       <c r="A19" s="94">
         <v>50</v>
       </c>
-      <c r="B19" s="154" t="s">
+      <c r="B19" s="149" t="s">
         <v>183</v>
       </c>
       <c r="C19" s="27" t="s">
@@ -3583,7 +3825,7 @@
       <c r="A20" s="94">
         <v>60</v>
       </c>
-      <c r="B20" s="154" t="s">
+      <c r="B20" s="149" t="s">
         <v>184</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -3654,6 +3896,7 @@
   <hyperlinks>
     <hyperlink ref="B4" location="'SU A0100'!A1" display="'SU A0100'!A1"/>
     <hyperlink ref="E3" location="dSU_01005" display="Drawing"/>
+    <hyperlink ref="G2" location="SU_A0100_BOM" display="Back to BOM"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3699,8 +3942,8 @@
   </sheetPr>
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3739,7 +3982,7 @@
       <c r="D2" s="58"/>
       <c r="E2" s="58"/>
       <c r="F2" s="58"/>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="97" t="s">
         <v>127</v>
       </c>
       <c r="H2" s="58"/>
@@ -3981,11 +4224,11 @@
       <c r="C11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="161">
+      <c r="D11" s="156">
         <f>4.2</f>
         <v>4.2</v>
       </c>
-      <c r="E11" s="157">
+      <c r="E11" s="152">
         <f>J11*K11*L11/1000000000</f>
         <v>1.4715095040000001E-2</v>
       </c>
@@ -4010,7 +4253,7 @@
       <c r="M11" s="24">
         <v>1</v>
       </c>
-      <c r="N11" s="162">
+      <c r="N11" s="157">
         <f>D11*E11</f>
         <v>6.1803399168000005E-2</v>
       </c>
@@ -4054,7 +4297,7 @@
       <c r="M13" s="58"/>
       <c r="N13" s="58"/>
       <c r="O13" s="64"/>
-      <c r="Q13" s="155"/>
+      <c r="Q13" s="150"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="119" t="s">
@@ -4127,7 +4370,7 @@
       <c r="A16" s="66">
         <v>20</v>
       </c>
-      <c r="B16" s="154" t="s">
+      <c r="B16" s="149" t="s">
         <v>184</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -4139,7 +4382,7 @@
       <c r="E16" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="F16" s="160">
+      <c r="F16" s="155">
         <v>0.05</v>
       </c>
       <c r="G16" s="28"/>
@@ -4159,7 +4402,7 @@
       <c r="A17" s="94">
         <v>30</v>
       </c>
-      <c r="B17" s="154" t="s">
+      <c r="B17" s="149" t="s">
         <v>183</v>
       </c>
       <c r="C17" s="27" t="s">
@@ -4191,7 +4434,7 @@
       <c r="A18" s="66">
         <v>40</v>
       </c>
-      <c r="B18" s="154" t="s">
+      <c r="B18" s="149" t="s">
         <v>184</v>
       </c>
       <c r="C18" s="19" t="s">
@@ -4203,7 +4446,7 @@
       <c r="E18" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="F18" s="160">
+      <c r="F18" s="155">
         <v>0.05</v>
       </c>
       <c r="G18" s="28"/>
@@ -4262,8 +4505,10 @@
   <hyperlinks>
     <hyperlink ref="B4" location="'SU A0100'!A1" display="'SU A0100'!A1"/>
     <hyperlink ref="E3" location="dSU_01006" display="Drawing"/>
+    <hyperlink ref="G2" location="SU_A0100_BOM" display="Back to BOM"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4315,11 +4560,11 @@
   <dimension ref="A1:O164"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H10" sqref="H10"/>
       <selection pane="topRight" activeCell="H10" sqref="H10"/>
       <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4447,352 +4692,459 @@
         <f>[1]SU_A0200!B3</f>
         <v>Suspension &amp; Shocks</v>
       </c>
-      <c r="C7" s="123" t="e">
-        <f>EL_A0001</f>
-        <v>#NAME?</v>
+      <c r="C7" s="130" t="str">
+        <f>SU_A0100</f>
+        <v>SU A0100</v>
       </c>
       <c r="D7" s="123" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="123"/>
-      <c r="F7" s="124" t="str">
-        <f>[1]SU_A0200!B4</f>
-        <v>Lower Front A-arm</v>
+      <c r="F7" s="173" t="str">
+        <f>'SU A0100'!B4</f>
+        <v>Upper Front A-arm</v>
       </c>
       <c r="G7" s="123"/>
-      <c r="H7" s="125" t="e">
+      <c r="H7" s="124">
         <f t="shared" ref="H7:H17" si="0">SUM(J7:M7)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="I7" s="126" t="e">
-        <f>BR_A0001_q</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J7" s="127" t="e">
-        <f>BR_A0001_m</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K7" s="127" t="e">
-        <f>BR_A0001_p</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L7" s="127" t="e">
-        <f>BR_A0001_f</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M7" s="127" t="e">
-        <f>BR_A0001_t</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N7" s="128" t="e">
+        <v>30.137392541559642</v>
+      </c>
+      <c r="I7" s="136">
+        <f>SU_A0100_q</f>
+        <v>2</v>
+      </c>
+      <c r="J7" s="125">
+        <f>SU_A0100_m</f>
+        <v>20.759999999999998</v>
+      </c>
+      <c r="K7" s="125">
+        <f>SU_A0100_p</f>
+        <v>8.595516447372308</v>
+      </c>
+      <c r="L7" s="125">
+        <f>SU_A0100_f</f>
+        <v>0.78187609418733417</v>
+      </c>
+      <c r="M7" s="125">
+        <v>0</v>
+      </c>
+      <c r="N7" s="126">
         <f t="shared" ref="N7:N17" si="1">H7*I7</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="O7" s="129"/>
+        <v>60.274785083119284</v>
+      </c>
+      <c r="O7" s="127"/>
     </row>
     <row r="8" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="130"/>
-      <c r="B8" s="131" t="str">
+      <c r="A8" s="128"/>
+      <c r="B8" s="129" t="str">
         <f>[1]SU_A0200!B3</f>
         <v>Suspension &amp; Shocks</v>
       </c>
-      <c r="C8" s="132" t="e">
-        <f>EL_01001</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="D8" s="133" t="s">
+      <c r="C8" s="130" t="str">
+        <f>SU_01001</f>
+        <v>SU_01001</v>
+      </c>
+      <c r="D8" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="133" t="str">
-        <f>F7</f>
-        <v>Lower Front A-arm</v>
-      </c>
-      <c r="F8" s="134" t="str">
-        <f>[1]SU_02001!B5</f>
-        <v>Lower Front Bearing Support</v>
-      </c>
-      <c r="G8" s="133"/>
-      <c r="H8" s="135" t="e">
+      <c r="E8" s="130" t="str">
+        <f>$F$7</f>
+        <v>Upper Front A-arm</v>
+      </c>
+      <c r="F8" s="131" t="str">
+        <f>'SU 01001'!B5</f>
+        <v>Upper Front Bearing Support</v>
+      </c>
+      <c r="G8" s="130"/>
+      <c r="H8" s="132">
         <f t="shared" si="0"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="I8" s="136" t="e">
-        <f>BR_A0001_q*BR_01001_q</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="J8" s="137" t="e">
-        <f>BR_01001_m</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K8" s="137" t="e">
-        <f>BR_01001_p</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L8" s="137" t="e">
-        <f>BR_01001_f</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M8" s="137" t="e">
-        <f>BR_01001_t</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N8" s="138" t="e">
+        <v>19.08406304</v>
+      </c>
+      <c r="I8" s="136">
+        <f>SU_A0100_q*SU_01001_q</f>
+        <v>4</v>
+      </c>
+      <c r="J8" s="133">
+        <f>SU_01001_m</f>
+        <v>4.2440630400000003</v>
+      </c>
+      <c r="K8" s="133">
+        <f>SU_01001_p</f>
+        <v>14.84</v>
+      </c>
+      <c r="L8" s="133">
+        <v>0</v>
+      </c>
+      <c r="M8" s="125">
+        <v>0</v>
+      </c>
+      <c r="N8" s="134">
         <f t="shared" si="1"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="O8" s="139"/>
-    </row>
-    <row r="9" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A9" s="130"/>
-      <c r="B9" s="131" t="str">
+        <v>76.336252160000001</v>
+      </c>
+      <c r="O8" s="135"/>
+    </row>
+    <row r="9" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="128"/>
+      <c r="B9" s="129" t="str">
         <f>[1]SU_A0200!$B$3</f>
         <v>Suspension &amp; Shocks</v>
       </c>
-      <c r="C9" s="133"/>
-      <c r="D9" s="133" t="s">
+      <c r="C9" s="130" t="str">
+        <f>SU_01002</f>
+        <v>SU_01002</v>
+      </c>
+      <c r="D9" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="133"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="133"/>
-      <c r="H9" s="135">
+      <c r="E9" s="130" t="str">
+        <f t="shared" ref="E9:E13" si="2">$F$7</f>
+        <v>Upper Front A-arm</v>
+      </c>
+      <c r="F9" s="131" t="str">
+        <f>'SU 01002'!B5</f>
+        <v>Inner Bearing Support</v>
+      </c>
+      <c r="G9" s="130"/>
+      <c r="H9" s="132">
+        <f t="shared" si="0"/>
+        <v>4.6183805439999999</v>
+      </c>
+      <c r="I9" s="136">
+        <f>SU_A0100_q*SU_01002_q</f>
+        <v>8</v>
+      </c>
+      <c r="J9" s="133">
+        <f>SU_01002_m</f>
+        <v>0.85838054400000008</v>
+      </c>
+      <c r="K9" s="133">
+        <f>SU_01002_p</f>
+        <v>3.76</v>
+      </c>
+      <c r="L9" s="133">
+        <v>0</v>
+      </c>
+      <c r="M9" s="125">
+        <v>0</v>
+      </c>
+      <c r="N9" s="134">
+        <f t="shared" si="1"/>
+        <v>36.947044351999999</v>
+      </c>
+      <c r="O9" s="135"/>
+    </row>
+    <row r="10" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="128"/>
+      <c r="B10" s="129" t="str">
+        <f>[1]SU_A0200!$B$3</f>
+        <v>Suspension &amp; Shocks</v>
+      </c>
+      <c r="C10" s="130" t="str">
+        <f>SU_01003</f>
+        <v>SU_01003</v>
+      </c>
+      <c r="D10" s="130" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="130" t="str">
+        <f t="shared" si="2"/>
+        <v>Upper Front A-arm</v>
+      </c>
+      <c r="F10" s="131" t="str">
+        <f>'SU 01003'!B5</f>
+        <v>Upper Front A-arm tube (Front)  Carbon Fiber Tube</v>
+      </c>
+      <c r="G10" s="130"/>
+      <c r="H10" s="132">
+        <f t="shared" si="0"/>
+        <v>230.06737599999997</v>
+      </c>
+      <c r="I10" s="136">
+        <f>SU_A0100_q*SU_01003_q</f>
+        <v>4</v>
+      </c>
+      <c r="J10" s="133">
+        <f>SU_01003_m</f>
+        <v>229.71737599999997</v>
+      </c>
+      <c r="K10" s="133">
+        <f>SU_01003_p</f>
+        <v>0.35</v>
+      </c>
+      <c r="L10" s="133">
+        <v>0</v>
+      </c>
+      <c r="M10" s="125">
+        <v>0</v>
+      </c>
+      <c r="N10" s="134">
+        <f t="shared" si="1"/>
+        <v>920.26950399999987</v>
+      </c>
+      <c r="O10" s="135"/>
+    </row>
+    <row r="11" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="128"/>
+      <c r="B11" s="129" t="str">
+        <f>[1]SU_A0200!$B$3</f>
+        <v>Suspension &amp; Shocks</v>
+      </c>
+      <c r="C11" s="130" t="str">
+        <f>SU_01004</f>
+        <v>SU_01004</v>
+      </c>
+      <c r="D11" s="130" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="130" t="str">
+        <f t="shared" si="2"/>
+        <v>Upper Front A-arm</v>
+      </c>
+      <c r="F11" s="131" t="str">
+        <f>'SU 01004'!B5</f>
+        <v>Upper Front A-arm tube (Back)  Carbon Fiber Tube</v>
+      </c>
+      <c r="G11" s="130"/>
+      <c r="H11" s="132">
+        <f t="shared" si="0"/>
+        <v>186.38872000000001</v>
+      </c>
+      <c r="I11" s="136">
+        <f>SU_A0100_q*SU_01004_q</f>
+        <v>4</v>
+      </c>
+      <c r="J11" s="133">
+        <f>SU_01004_m</f>
+        <v>186.03872000000001</v>
+      </c>
+      <c r="K11" s="133">
+        <f>SU_01004_p</f>
+        <v>0.35</v>
+      </c>
+      <c r="L11" s="133">
+        <v>0</v>
+      </c>
+      <c r="M11" s="125">
+        <v>0</v>
+      </c>
+      <c r="N11" s="134">
+        <f t="shared" si="1"/>
+        <v>745.55488000000003</v>
+      </c>
+      <c r="O11" s="135"/>
+    </row>
+    <row r="12" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="128"/>
+      <c r="B12" s="129" t="str">
+        <f>[1]SU_A0200!$B$3</f>
+        <v>Suspension &amp; Shocks</v>
+      </c>
+      <c r="C12" s="130" t="str">
+        <f>SU_01005</f>
+        <v>SU_01005</v>
+      </c>
+      <c r="D12" s="130" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="130" t="str">
+        <f t="shared" si="2"/>
+        <v>Upper Front A-arm</v>
+      </c>
+      <c r="F12" s="131" t="str">
+        <f>'SU 01005'!B5</f>
+        <v>Spacer</v>
+      </c>
+      <c r="G12" s="130"/>
+      <c r="H12" s="132">
+        <f t="shared" si="0"/>
+        <v>2.6754945600000002</v>
+      </c>
+      <c r="I12" s="136">
+        <f>SU_A0100_q*SU_01005_q</f>
+        <v>24</v>
+      </c>
+      <c r="J12" s="133">
+        <f>SU_01005_m</f>
+        <v>3.5494560000000008E-2</v>
+      </c>
+      <c r="K12" s="133">
+        <f>SU_01005_p</f>
+        <v>2.64</v>
+      </c>
+      <c r="L12" s="133">
+        <v>0</v>
+      </c>
+      <c r="M12" s="125">
+        <v>0</v>
+      </c>
+      <c r="N12" s="134">
+        <f t="shared" si="1"/>
+        <v>64.211869440000001</v>
+      </c>
+      <c r="O12" s="135"/>
+    </row>
+    <row r="13" spans="1:15" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="128"/>
+      <c r="B13" s="129" t="str">
+        <f>[1]SU_A0200!$B$3</f>
+        <v>Suspension &amp; Shocks</v>
+      </c>
+      <c r="C13" s="130" t="str">
+        <f>SU_01006</f>
+        <v>SU_01006</v>
+      </c>
+      <c r="D13" s="130" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="130" t="str">
+        <f t="shared" si="2"/>
+        <v>Upper Front A-arm</v>
+      </c>
+      <c r="F13" s="131" t="str">
+        <f>'SU 01006'!$B$5</f>
+        <v>Outboard A-arm Insert</v>
+      </c>
+      <c r="G13" s="130"/>
+      <c r="H13" s="132">
+        <f t="shared" si="0"/>
+        <v>2.015803399168</v>
+      </c>
+      <c r="I13" s="136">
+        <f>SU_A0100_q*SU_01006_q</f>
+        <v>8</v>
+      </c>
+      <c r="J13" s="133">
+        <f>SU_01006_m</f>
+        <v>6.1803399168000005E-2</v>
+      </c>
+      <c r="K13" s="133">
+        <f>SU_01006_p</f>
+        <v>1.954</v>
+      </c>
+      <c r="L13" s="133">
+        <v>0</v>
+      </c>
+      <c r="M13" s="125">
+        <v>0</v>
+      </c>
+      <c r="N13" s="134">
+        <f t="shared" si="1"/>
+        <v>16.126427193344</v>
+      </c>
+      <c r="O13" s="135"/>
+    </row>
+    <row r="14" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="128"/>
+      <c r="B14" s="129" t="str">
+        <f>[1]SU_A0200!$B$3</f>
+        <v>Suspension &amp; Shocks</v>
+      </c>
+      <c r="C14" s="130"/>
+      <c r="D14" s="130" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="130"/>
+      <c r="F14" s="129"/>
+      <c r="G14" s="130"/>
+      <c r="H14" s="132">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="140"/>
-      <c r="J9" s="137"/>
-      <c r="K9" s="137"/>
-      <c r="L9" s="137"/>
-      <c r="M9" s="137"/>
-      <c r="N9" s="138">
+      <c r="I14" s="136"/>
+      <c r="J14" s="133"/>
+      <c r="K14" s="133"/>
+      <c r="L14" s="133"/>
+      <c r="M14" s="133"/>
+      <c r="N14" s="134">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O9" s="139"/>
-    </row>
-    <row r="10" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
-      <c r="B10" s="131" t="str">
+      <c r="O14" s="135"/>
+    </row>
+    <row r="15" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="128"/>
+      <c r="B15" s="129" t="str">
         <f>[1]SU_A0200!$B$3</f>
         <v>Suspension &amp; Shocks</v>
       </c>
-      <c r="C10" s="133"/>
-      <c r="D10" s="133" t="s">
+      <c r="C15" s="130"/>
+      <c r="D15" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="133"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="133"/>
-      <c r="H10" s="135">
+      <c r="E15" s="130"/>
+      <c r="F15" s="129"/>
+      <c r="G15" s="137"/>
+      <c r="H15" s="132">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I10" s="140"/>
-      <c r="J10" s="137"/>
-      <c r="K10" s="137"/>
-      <c r="L10" s="137"/>
-      <c r="M10" s="137"/>
-      <c r="N10" s="138">
+      <c r="I15" s="136"/>
+      <c r="J15" s="133"/>
+      <c r="K15" s="133"/>
+      <c r="L15" s="133"/>
+      <c r="M15" s="133"/>
+      <c r="N15" s="134">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O10" s="139"/>
-    </row>
-    <row r="11" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="130"/>
-      <c r="B11" s="131" t="str">
+      <c r="O15" s="135"/>
+    </row>
+    <row r="16" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="128"/>
+      <c r="B16" s="129" t="str">
         <f>[1]SU_A0200!$B$3</f>
         <v>Suspension &amp; Shocks</v>
       </c>
-      <c r="C11" s="133"/>
-      <c r="D11" s="133" t="s">
+      <c r="C16" s="130"/>
+      <c r="D16" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="133"/>
-      <c r="F11" s="131"/>
-      <c r="G11" s="133"/>
-      <c r="H11" s="135">
+      <c r="E16" s="130"/>
+      <c r="F16" s="129"/>
+      <c r="G16" s="130"/>
+      <c r="H16" s="132">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I11" s="140"/>
-      <c r="J11" s="137"/>
-      <c r="K11" s="137"/>
-      <c r="L11" s="137"/>
-      <c r="M11" s="137"/>
-      <c r="N11" s="138">
+      <c r="I16" s="136"/>
+      <c r="J16" s="133"/>
+      <c r="K16" s="133"/>
+      <c r="L16" s="133"/>
+      <c r="M16" s="133"/>
+      <c r="N16" s="134">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O11" s="139"/>
-    </row>
-    <row r="12" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="130"/>
-      <c r="B12" s="131" t="str">
+      <c r="O16" s="135"/>
+    </row>
+    <row r="17" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="128"/>
+      <c r="B17" s="129" t="str">
         <f>[1]SU_A0200!$B$3</f>
         <v>Suspension &amp; Shocks</v>
       </c>
-      <c r="C12" s="133"/>
-      <c r="D12" s="133" t="s">
+      <c r="C17" s="130"/>
+      <c r="D17" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="133"/>
-      <c r="F12" s="131"/>
-      <c r="G12" s="133"/>
-      <c r="H12" s="135">
+      <c r="E17" s="130"/>
+      <c r="F17" s="129"/>
+      <c r="G17" s="130"/>
+      <c r="H17" s="132">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I12" s="140"/>
-      <c r="J12" s="137"/>
-      <c r="K12" s="137"/>
-      <c r="L12" s="137"/>
-      <c r="M12" s="137"/>
-      <c r="N12" s="138">
+      <c r="I17" s="136"/>
+      <c r="J17" s="133"/>
+      <c r="K17" s="133"/>
+      <c r="L17" s="133"/>
+      <c r="M17" s="133"/>
+      <c r="N17" s="134">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O12" s="139"/>
-    </row>
-    <row r="13" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="130"/>
-      <c r="B13" s="131" t="str">
-        <f>[1]SU_A0200!$B$3</f>
-        <v>Suspension &amp; Shocks</v>
-      </c>
-      <c r="C13" s="133"/>
-      <c r="D13" s="133" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="133"/>
-      <c r="F13" s="131"/>
-      <c r="G13" s="133"/>
-      <c r="H13" s="135">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13" s="140"/>
-      <c r="J13" s="137"/>
-      <c r="K13" s="137"/>
-      <c r="L13" s="137"/>
-      <c r="M13" s="137"/>
-      <c r="N13" s="138">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="139"/>
-    </row>
-    <row r="14" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="130"/>
-      <c r="B14" s="131" t="str">
-        <f>[1]SU_A0200!$B$3</f>
-        <v>Suspension &amp; Shocks</v>
-      </c>
-      <c r="C14" s="133"/>
-      <c r="D14" s="133" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="133"/>
-      <c r="F14" s="131"/>
-      <c r="G14" s="133"/>
-      <c r="H14" s="135">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14" s="140"/>
-      <c r="J14" s="137"/>
-      <c r="K14" s="137"/>
-      <c r="L14" s="137"/>
-      <c r="M14" s="137"/>
-      <c r="N14" s="138">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="139"/>
-    </row>
-    <row r="15" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="130"/>
-      <c r="B15" s="131" t="str">
-        <f>[1]SU_A0200!$B$3</f>
-        <v>Suspension &amp; Shocks</v>
-      </c>
-      <c r="C15" s="133"/>
-      <c r="D15" s="133" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="133"/>
-      <c r="F15" s="131"/>
-      <c r="G15" s="141"/>
-      <c r="H15" s="135">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="140"/>
-      <c r="J15" s="137"/>
-      <c r="K15" s="137"/>
-      <c r="L15" s="137"/>
-      <c r="M15" s="137"/>
-      <c r="N15" s="138">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O15" s="139"/>
-    </row>
-    <row r="16" spans="1:15" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="130"/>
-      <c r="B16" s="131" t="str">
-        <f>[1]SU_A0200!$B$3</f>
-        <v>Suspension &amp; Shocks</v>
-      </c>
-      <c r="C16" s="133"/>
-      <c r="D16" s="133" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="133"/>
-      <c r="F16" s="131"/>
-      <c r="G16" s="133"/>
-      <c r="H16" s="135">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="140"/>
-      <c r="J16" s="137"/>
-      <c r="K16" s="137"/>
-      <c r="L16" s="137"/>
-      <c r="M16" s="137"/>
-      <c r="N16" s="138">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="139"/>
-    </row>
-    <row r="17" spans="1:15" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="130"/>
-      <c r="B17" s="131" t="str">
-        <f>[1]SU_A0200!$B$3</f>
-        <v>Suspension &amp; Shocks</v>
-      </c>
-      <c r="C17" s="133"/>
-      <c r="D17" s="133" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="133"/>
-      <c r="F17" s="131"/>
-      <c r="G17" s="133"/>
-      <c r="H17" s="135">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I17" s="140"/>
-      <c r="J17" s="137"/>
-      <c r="K17" s="137"/>
-      <c r="L17" s="137"/>
-      <c r="M17" s="137"/>
-      <c r="N17" s="138">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O17" s="139"/>
+      <c r="O17" s="135"/>
     </row>
     <row r="18" spans="1:15" s="12" customFormat="1" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
@@ -4809,25 +5161,25 @@
       <c r="G18" s="1"/>
       <c r="H18" s="3"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="105" t="e">
+      <c r="J18" s="105">
         <f>SUMPRODUCT($I7:$I17,J7:J17)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="K18" s="105" t="e">
+        <v>1729.7339771453439</v>
+      </c>
+      <c r="K18" s="105">
         <f>SUMPRODUCT($I7:$I17,K7:K17)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="L18" s="105" t="e">
+        <v>188.42303289474464</v>
+      </c>
+      <c r="L18" s="105">
         <f>SUMPRODUCT($I7:$I17,L7:L17)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="M18" s="105" t="e">
+        <v>1.5637521883746683</v>
+      </c>
+      <c r="M18" s="105">
         <f>SUMPRODUCT($I7:$I17,M7:M17)</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="N18" s="105" t="e">
+        <v>0</v>
+      </c>
+      <c r="N18" s="105">
         <f>SUM(N7:N17)</f>
-        <v>#NAME?</v>
+        <v>1919.7207622284634</v>
       </c>
       <c r="O18" s="2"/>
     </row>
@@ -7053,8 +7405,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F7" location="BR_A0001" display="BR_A0001"/>
-    <hyperlink ref="F8" location="BR_01001" display="BR_01001"/>
+    <hyperlink ref="F7" location="'SU A0100'!A1" display="'SU A0100'!A1"/>
+    <hyperlink ref="F8" location="SU_01001" display="SU_01001"/>
+    <hyperlink ref="F9" location="SU_01002" display="SU_01002"/>
+    <hyperlink ref="F10" location="SU_01003" display="SU_01003"/>
+    <hyperlink ref="F11" location="SU_01004" display="SU_01004"/>
+    <hyperlink ref="F12" location="SU_01005" display="SU_01005"/>
+    <hyperlink ref="F13" location="SU_01006" display="SU_01006"/>
   </hyperlinks>
   <pageMargins left="0.41" right="0.22" top="0.72" bottom="0.57999999999999996" header="0.5" footer="0.26"/>
   <pageSetup scale="57" fitToHeight="99" orientation="landscape" r:id="rId1"/>
@@ -7073,16 +7430,16 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A7" zoomScale="68" zoomScaleNormal="68" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="57.109375" customWidth="1"/>
-    <col min="3" max="3" width="55.6640625" customWidth="1"/>
+    <col min="3" max="3" width="48.21875" customWidth="1"/>
     <col min="5" max="5" width="14.109375" customWidth="1"/>
-    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="14" max="14" width="13.77734375" customWidth="1"/>
     <col min="15" max="15" width="5.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7112,7 +7469,7 @@
       </c>
       <c r="C2" s="58"/>
       <c r="D2" s="58"/>
-      <c r="E2" s="58" t="s">
+      <c r="E2" s="97" t="s">
         <v>127</v>
       </c>
       <c r="F2" s="58"/>
@@ -7307,7 +7664,7 @@
         <f>'SU 01001'!N2</f>
         <v>19.08406304</v>
       </c>
-      <c r="D10" s="144">
+      <c r="D10" s="140">
         <v>1</v>
       </c>
       <c r="E10" s="77">
@@ -7341,7 +7698,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="77">
-        <f t="shared" ref="E10:E15" si="0">C11*D11</f>
+        <f t="shared" ref="E11:E15" si="0">C11*D11</f>
         <v>9.2367610879999997</v>
       </c>
       <c r="F11" s="59"/>
@@ -7457,7 +7814,7 @@
         <f>'SU 01006'!N2</f>
         <v>2.015803399168</v>
       </c>
-      <c r="D15" s="143">
+      <c r="D15" s="139">
         <v>2</v>
       </c>
       <c r="E15" s="77">
@@ -7567,7 +7924,7 @@
         <v>132</v>
       </c>
       <c r="C19" s="75"/>
-      <c r="D19" s="142">
+      <c r="D19" s="138">
         <f>0.03*E19^2+5</f>
         <v>6.92</v>
       </c>
@@ -7596,10 +7953,10 @@
       <c r="A20" s="75">
         <v>20</v>
       </c>
-      <c r="B20" s="164" t="s">
+      <c r="B20" s="159" t="s">
         <v>137</v>
       </c>
-      <c r="C20" s="165" t="s">
+      <c r="C20" s="160" t="s">
         <v>138</v>
       </c>
       <c r="D20" s="77"/>
@@ -7620,14 +7977,14 @@
       </c>
       <c r="O20" s="69"/>
     </row>
-    <row r="21" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="75">
         <v>30</v>
       </c>
-      <c r="B21" s="164" t="s">
+      <c r="B21" s="159" t="s">
         <v>137</v>
       </c>
-      <c r="C21" s="165" t="s">
+      <c r="C21" s="160" t="s">
         <v>139</v>
       </c>
       <c r="D21" s="77"/>
@@ -7721,28 +8078,28 @@
       <c r="O24" s="71"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="164">
+      <c r="A25" s="159">
         <v>10</v>
       </c>
-      <c r="B25" s="166" t="s">
+      <c r="B25" s="161" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="166" t="s">
+      <c r="C25" s="161" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="145">
+      <c r="D25" s="141">
         <v>0.02</v>
       </c>
-      <c r="E25" s="164" t="s">
+      <c r="E25" s="159" t="s">
         <v>142</v>
       </c>
-      <c r="F25" s="167">
+      <c r="F25" s="162">
         <f>3*2*PI()*0.8*0.5</f>
         <v>7.5398223686155035</v>
       </c>
-      <c r="G25" s="164"/>
-      <c r="H25" s="164"/>
-      <c r="I25" s="145">
+      <c r="G25" s="159"/>
+      <c r="H25" s="159"/>
+      <c r="I25" s="141">
         <f>D25*F25</f>
         <v>0.15079644737231007</v>
       </c>
@@ -7760,7 +8117,7 @@
       <c r="B26" s="88" t="s">
         <v>143</v>
       </c>
-      <c r="C26" s="166" t="s">
+      <c r="C26" s="161" t="s">
         <v>144</v>
       </c>
       <c r="D26" s="77">
@@ -7789,7 +8146,7 @@
       <c r="A27" s="75">
         <v>30</v>
       </c>
-      <c r="B27" s="146" t="s">
+      <c r="B27" s="142" t="s">
         <v>145</v>
       </c>
       <c r="C27" s="75" t="s">
@@ -7821,7 +8178,7 @@
       <c r="A28" s="75">
         <v>40</v>
       </c>
-      <c r="B28" s="146" t="s">
+      <c r="B28" s="142" t="s">
         <v>145</v>
       </c>
       <c r="C28" s="75" t="s">
@@ -7853,7 +8210,7 @@
       <c r="A29" s="75">
         <v>50</v>
       </c>
-      <c r="B29" s="146" t="s">
+      <c r="B29" s="142" t="s">
         <v>148</v>
       </c>
       <c r="C29" s="75" t="s">
@@ -7914,7 +8271,7 @@
       <c r="O30" s="68"/>
     </row>
     <row r="31" spans="1:15" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="164">
+      <c r="A31" s="159">
         <v>70</v>
       </c>
       <c r="B31" s="88" t="s">
@@ -7981,7 +8338,7 @@
       <c r="A33" s="75">
         <v>90</v>
       </c>
-      <c r="B33" s="147" t="s">
+      <c r="B33" s="88" t="s">
         <v>153</v>
       </c>
       <c r="C33" s="75" t="s">
@@ -8014,7 +8371,7 @@
       <c r="A34" s="75">
         <v>100</v>
       </c>
-      <c r="B34" s="147" t="s">
+      <c r="B34" s="88" t="s">
         <v>157</v>
       </c>
       <c r="C34" s="75" t="s">
@@ -8047,19 +8404,19 @@
       <c r="A35" s="75">
         <v>110</v>
       </c>
-      <c r="B35" s="166" t="s">
+      <c r="B35" s="161" t="s">
         <v>158</v>
       </c>
-      <c r="C35" s="166" t="s">
+      <c r="C35" s="161" t="s">
         <v>159</v>
       </c>
-      <c r="D35" s="145">
+      <c r="D35" s="141">
         <v>0.06</v>
       </c>
-      <c r="E35" s="164" t="s">
+      <c r="E35" s="159" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="164">
+      <c r="F35" s="159">
         <v>1</v>
       </c>
       <c r="G35" s="75"/>
@@ -8079,19 +8436,19 @@
       <c r="A36" s="75">
         <v>120</v>
       </c>
-      <c r="B36" s="168" t="s">
+      <c r="B36" s="163" t="s">
         <v>160</v>
       </c>
-      <c r="C36" s="168" t="s">
+      <c r="C36" s="163" t="s">
         <v>161</v>
       </c>
-      <c r="D36" s="148">
+      <c r="D36" s="143">
         <v>0.13</v>
       </c>
-      <c r="E36" s="169" t="s">
+      <c r="E36" s="164" t="s">
         <v>32</v>
       </c>
-      <c r="F36" s="169">
+      <c r="F36" s="164">
         <v>4</v>
       </c>
       <c r="G36" s="75"/>
@@ -8111,19 +8468,19 @@
       <c r="A37" s="75">
         <v>130</v>
       </c>
-      <c r="B37" s="170" t="s">
+      <c r="B37" s="165" t="s">
         <v>160</v>
       </c>
-      <c r="C37" s="170" t="s">
+      <c r="C37" s="165" t="s">
         <v>162</v>
       </c>
-      <c r="D37" s="149">
+      <c r="D37" s="144">
         <v>0.13</v>
       </c>
-      <c r="E37" s="171" t="s">
+      <c r="E37" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="F37" s="171">
+      <c r="F37" s="166">
         <v>4</v>
       </c>
       <c r="G37" s="75"/>
@@ -8143,19 +8500,19 @@
       <c r="A38" s="75">
         <v>140</v>
       </c>
-      <c r="B38" s="170" t="s">
+      <c r="B38" s="165" t="s">
         <v>158</v>
       </c>
-      <c r="C38" s="170" t="s">
+      <c r="C38" s="165" t="s">
         <v>163</v>
       </c>
-      <c r="D38" s="149">
+      <c r="D38" s="144">
         <v>0.06</v>
       </c>
-      <c r="E38" s="171" t="s">
+      <c r="E38" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="F38" s="171">
+      <c r="F38" s="166">
         <v>1</v>
       </c>
       <c r="G38" s="75"/>
@@ -8175,19 +8532,19 @@
       <c r="A39" s="75">
         <v>150</v>
       </c>
-      <c r="B39" s="170" t="s">
+      <c r="B39" s="165" t="s">
         <v>160</v>
       </c>
-      <c r="C39" s="170" t="s">
+      <c r="C39" s="165" t="s">
         <v>164</v>
       </c>
-      <c r="D39" s="149">
+      <c r="D39" s="144">
         <v>0.13</v>
       </c>
-      <c r="E39" s="171" t="s">
+      <c r="E39" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="171">
+      <c r="F39" s="166">
         <v>2</v>
       </c>
       <c r="G39" s="75"/>
@@ -8207,19 +8564,19 @@
       <c r="A40" s="75">
         <v>160</v>
       </c>
-      <c r="B40" s="170" t="s">
+      <c r="B40" s="165" t="s">
         <v>160</v>
       </c>
-      <c r="C40" s="170" t="s">
+      <c r="C40" s="165" t="s">
         <v>165</v>
       </c>
-      <c r="D40" s="149">
+      <c r="D40" s="144">
         <v>0.13</v>
       </c>
-      <c r="E40" s="171" t="s">
+      <c r="E40" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="F40" s="171">
+      <c r="F40" s="166">
         <v>2</v>
       </c>
       <c r="G40" s="75"/>
@@ -8239,19 +8596,19 @@
       <c r="A41" s="75">
         <v>170</v>
       </c>
-      <c r="B41" s="172" t="s">
+      <c r="B41" s="167" t="s">
         <v>166</v>
       </c>
-      <c r="C41" s="173" t="s">
+      <c r="C41" s="168" t="s">
         <v>167</v>
       </c>
-      <c r="D41" s="149">
+      <c r="D41" s="144">
         <v>0.75</v>
       </c>
-      <c r="E41" s="171" t="s">
+      <c r="E41" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="F41" s="171">
+      <c r="F41" s="166">
         <v>3</v>
       </c>
       <c r="G41" s="87"/>
@@ -8271,19 +8628,19 @@
       <c r="A42" s="75">
         <v>180</v>
       </c>
-      <c r="B42" s="172" t="s">
+      <c r="B42" s="167" t="s">
         <v>168</v>
       </c>
-      <c r="C42" s="173" t="s">
+      <c r="C42" s="168" t="s">
         <v>169</v>
       </c>
-      <c r="D42" s="149">
+      <c r="D42" s="144">
         <v>0.25</v>
       </c>
-      <c r="E42" s="173" t="s">
+      <c r="E42" s="168" t="s">
         <v>32</v>
       </c>
-      <c r="F42" s="171">
+      <c r="F42" s="166">
         <v>3</v>
       </c>
       <c r="G42" s="75"/>
@@ -8376,35 +8733,35 @@
       <c r="O45" s="64"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A46" s="164">
+      <c r="A46" s="159">
         <v>10</v>
       </c>
-      <c r="B46" s="164" t="s">
+      <c r="B46" s="159" t="s">
         <v>170</v>
       </c>
-      <c r="C46" s="164" t="s">
+      <c r="C46" s="159" t="s">
         <v>171</v>
       </c>
-      <c r="D46" s="174">
+      <c r="D46" s="169">
         <f>0.8/105154*E46^2*G46*SQRT(G46)+(0.003*EXP(0.319*E46))</f>
         <v>0.16167651505774214</v>
       </c>
-      <c r="E46" s="164">
+      <c r="E46" s="159">
         <v>8</v>
       </c>
-      <c r="F46" s="150" t="s">
+      <c r="F46" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="G46" s="175">
+      <c r="G46" s="170">
         <v>40</v>
       </c>
-      <c r="H46" s="166" t="s">
+      <c r="H46" s="161" t="s">
         <v>30</v>
       </c>
-      <c r="I46" s="151">
+      <c r="I46" s="146">
         <v>2</v>
       </c>
-      <c r="J46" s="152">
+      <c r="J46" s="147">
         <f>D46*I46</f>
         <v>0.32335303011548427</v>
       </c>
@@ -8415,35 +8772,35 @@
       <c r="O46" s="64"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" s="164">
+      <c r="A47" s="159">
         <v>20</v>
       </c>
-      <c r="B47" s="164" t="s">
+      <c r="B47" s="159" t="s">
         <v>170</v>
       </c>
-      <c r="C47" s="164" t="s">
+      <c r="C47" s="159" t="s">
         <v>172</v>
       </c>
-      <c r="D47" s="174">
+      <c r="D47" s="169">
         <f>0.8/105154*E47^2*G47*SQRT(G47)+(0.003*EXP(0.319*E47))</f>
         <v>0.26479118861318168</v>
       </c>
-      <c r="E47" s="164">
+      <c r="E47" s="159">
         <v>8</v>
       </c>
-      <c r="F47" s="150" t="s">
+      <c r="F47" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="G47" s="175">
+      <c r="G47" s="170">
         <v>60</v>
       </c>
-      <c r="H47" s="166" t="s">
+      <c r="H47" s="161" t="s">
         <v>30</v>
       </c>
-      <c r="I47" s="153">
+      <c r="I47" s="148">
         <v>1</v>
       </c>
-      <c r="J47" s="145">
+      <c r="J47" s="141">
         <f>D47*I47</f>
         <v>0.26479118861318168</v>
       </c>
@@ -8454,31 +8811,31 @@
       <c r="O47" s="64"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A48" s="164">
+      <c r="A48" s="159">
         <v>30</v>
       </c>
-      <c r="B48" s="164" t="s">
+      <c r="B48" s="159" t="s">
         <v>173</v>
       </c>
-      <c r="C48" s="164" t="s">
+      <c r="C48" s="159" t="s">
         <v>174</v>
       </c>
-      <c r="D48" s="176">
+      <c r="D48" s="171">
         <f>(0.009*EXP(0.2*E48))</f>
         <v>4.4577291819556032E-2</v>
       </c>
-      <c r="E48" s="164">
+      <c r="E48" s="159">
         <v>8</v>
       </c>
-      <c r="F48" s="150" t="s">
+      <c r="F48" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="G48" s="164"/>
-      <c r="H48" s="166"/>
-      <c r="I48" s="153">
+      <c r="G48" s="159"/>
+      <c r="H48" s="161"/>
+      <c r="I48" s="148">
         <v>3</v>
       </c>
-      <c r="J48" s="145">
+      <c r="J48" s="141">
         <f>D48*I48</f>
         <v>0.1337318754586681</v>
       </c>
@@ -8489,30 +8846,30 @@
       <c r="O48" s="64"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A49" s="164">
+      <c r="A49" s="159">
         <v>40</v>
       </c>
-      <c r="B49" s="164" t="s">
+      <c r="B49" s="159" t="s">
         <v>175</v>
       </c>
-      <c r="C49" s="164" t="s">
+      <c r="C49" s="159" t="s">
         <v>176</v>
       </c>
-      <c r="D49" s="164">
+      <c r="D49" s="159">
         <v>0.01</v>
       </c>
-      <c r="E49" s="164">
+      <c r="E49" s="159">
         <v>8</v>
       </c>
-      <c r="F49" s="150" t="s">
+      <c r="F49" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="G49" s="164"/>
-      <c r="H49" s="166"/>
-      <c r="I49" s="153">
+      <c r="G49" s="159"/>
+      <c r="H49" s="161"/>
+      <c r="I49" s="148">
         <v>6</v>
       </c>
-      <c r="J49" s="145">
+      <c r="J49" s="141">
         <f>D49*I49</f>
         <v>0.06</v>
       </c>
@@ -8603,6 +8960,7 @@
     <hyperlink ref="B11" location="SU_01002" display="SU_01002"/>
     <hyperlink ref="B12" location="SU_01003" display="SU_01003"/>
     <hyperlink ref="B13" location="SU_01004" display="SU_01004"/>
+    <hyperlink ref="E2" location="SU_A0100_BOM" display="Back to BOM"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
   <pageSetup paperSize="9" scale="39" firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -8625,7 +8983,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8664,7 +9022,7 @@
       <c r="D2" s="58"/>
       <c r="E2" s="58"/>
       <c r="F2" s="58"/>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="97" t="s">
         <v>127</v>
       </c>
       <c r="H2" s="58"/>
@@ -8917,7 +9275,7 @@
       <c r="I11" s="22" t="s">
         <v>134</v>
       </c>
-      <c r="J11" s="177">
+      <c r="J11" s="172">
         <f>90*90</f>
         <v>8100</v>
       </c>
@@ -8974,7 +9332,7 @@
       <c r="M13" s="58"/>
       <c r="N13" s="58"/>
       <c r="O13" s="64"/>
-      <c r="S13" s="155"/>
+      <c r="S13" s="150"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="119" t="s">
@@ -9010,7 +9368,7 @@
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
       <c r="O14" s="64"/>
-      <c r="R14" s="155"/>
+      <c r="R14" s="150"/>
     </row>
     <row r="15" spans="1:19" s="26" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="93">
@@ -9048,7 +9406,7 @@
       <c r="A16" s="66">
         <v>20</v>
       </c>
-      <c r="B16" s="154" t="s">
+      <c r="B16" s="149" t="s">
         <v>184</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -9075,13 +9433,13 @@
       <c r="M16" s="58"/>
       <c r="N16" s="58"/>
       <c r="O16" s="64"/>
-      <c r="R16" s="155"/>
+      <c r="R16" s="150"/>
     </row>
     <row r="17" spans="1:18" s="17" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="94">
         <v>30</v>
       </c>
-      <c r="B17" s="154" t="s">
+      <c r="B17" s="149" t="s">
         <v>183</v>
       </c>
       <c r="C17" s="27" t="s">
@@ -9108,13 +9466,13 @@
       <c r="M17" s="59"/>
       <c r="N17" s="59"/>
       <c r="O17" s="68"/>
-      <c r="R17" s="156"/>
+      <c r="R17" s="151"/>
     </row>
     <row r="18" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="66">
         <v>40</v>
       </c>
-      <c r="B18" s="154" t="s">
+      <c r="B18" s="149" t="s">
         <v>184</v>
       </c>
       <c r="C18" s="19" t="s">
@@ -9141,13 +9499,13 @@
       <c r="M18" s="58"/>
       <c r="N18" s="58"/>
       <c r="O18" s="64"/>
-      <c r="R18" s="155"/>
+      <c r="R18" s="150"/>
     </row>
     <row r="19" spans="1:18" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="94">
         <v>50</v>
       </c>
-      <c r="B19" s="154" t="s">
+      <c r="B19" s="149" t="s">
         <v>183</v>
       </c>
       <c r="C19" s="27" t="s">
@@ -9174,13 +9532,13 @@
       <c r="M19" s="58"/>
       <c r="N19" s="58"/>
       <c r="O19" s="64"/>
-      <c r="R19" s="155"/>
+      <c r="R19" s="150"/>
     </row>
     <row r="20" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="94">
         <v>60</v>
       </c>
-      <c r="B20" s="154" t="s">
+      <c r="B20" s="149" t="s">
         <v>184</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -9251,6 +9609,7 @@
   <hyperlinks>
     <hyperlink ref="B4" location="'SU A0100'!A1" display="'SU A0100'!A1"/>
     <hyperlink ref="E3" location="dSU_01001" display="Drawing"/>
+    <hyperlink ref="G2" location="SU_A0100_BOM" display="Back to BOM"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" scale="43" firstPageNumber="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -9310,7 +9669,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9348,7 +9707,7 @@
       <c r="D2" s="58"/>
       <c r="E2" s="58"/>
       <c r="F2" s="58"/>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="97" t="s">
         <v>127</v>
       </c>
       <c r="H2" s="58"/>
@@ -9594,7 +9953,7 @@
         <f>4.2</f>
         <v>4.2</v>
       </c>
-      <c r="E11" s="157">
+      <c r="E11" s="152">
         <f>J11*K11*L11/1000000000</f>
         <v>0.20437632</v>
       </c>
@@ -9667,8 +10026,8 @@
       <c r="M13" s="58"/>
       <c r="N13" s="58"/>
       <c r="O13" s="64"/>
-      <c r="R13" s="155"/>
-      <c r="S13" s="155"/>
+      <c r="R13" s="150"/>
+      <c r="S13" s="150"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="119" t="s">
@@ -9704,7 +10063,7 @@
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
       <c r="O14" s="64"/>
-      <c r="R14" s="155"/>
+      <c r="R14" s="150"/>
     </row>
     <row r="15" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="93">
@@ -9739,14 +10098,14 @@
       <c r="O15" s="71"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="26"/>
-      <c r="R15" s="158"/>
+      <c r="R15" s="153"/>
       <c r="S15" s="26"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="66">
         <v>20</v>
       </c>
-      <c r="B16" s="154" t="s">
+      <c r="B16" s="149" t="s">
         <v>184</v>
       </c>
       <c r="C16" s="19" t="s">
@@ -9773,13 +10132,13 @@
       <c r="M16" s="58"/>
       <c r="N16" s="58"/>
       <c r="O16" s="64"/>
-      <c r="R16" s="155"/>
+      <c r="R16" s="150"/>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="94">
         <v>30</v>
       </c>
-      <c r="B17" s="154" t="s">
+      <c r="B17" s="149" t="s">
         <v>183</v>
       </c>
       <c r="C17" s="27" t="s">
@@ -9808,14 +10167,14 @@
       <c r="O17" s="68"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="17"/>
-      <c r="R17" s="156"/>
+      <c r="R17" s="151"/>
       <c r="S17" s="17"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="66">
         <v>40</v>
       </c>
-      <c r="B18" s="154" t="s">
+      <c r="B18" s="149" t="s">
         <v>184</v>
       </c>
       <c r="C18" s="19" t="s">
@@ -9842,13 +10201,13 @@
       <c r="M18" s="58"/>
       <c r="N18" s="58"/>
       <c r="O18" s="64"/>
-      <c r="R18" s="155"/>
+      <c r="R18" s="150"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="94">
         <v>50</v>
       </c>
-      <c r="B19" s="154" t="s">
+      <c r="B19" s="149" t="s">
         <v>183</v>
       </c>
       <c r="C19" s="27" t="s">
@@ -9875,13 +10234,13 @@
       <c r="M19" s="58"/>
       <c r="N19" s="58"/>
       <c r="O19" s="64"/>
-      <c r="R19" s="155"/>
+      <c r="R19" s="150"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="94">
         <v>60</v>
       </c>
-      <c r="B20" s="154" t="s">
+      <c r="B20" s="149" t="s">
         <v>184</v>
       </c>
       <c r="C20" s="19" t="s">
@@ -9952,6 +10311,7 @@
   <hyperlinks>
     <hyperlink ref="B4" location="'SU A0100'!A1" display="'SU A0100'!A1"/>
     <hyperlink ref="E3" location="dSU_01002" display="Drawing"/>
+    <hyperlink ref="G2" location="SU_A0100_BOM" display="Back to BOM"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -9983,7 +10343,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="163"/>
+      <c r="B6" s="158"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -10002,7 +10362,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10040,7 +10400,7 @@
       <c r="D2" s="58"/>
       <c r="E2" s="58"/>
       <c r="F2" s="58"/>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="97" t="s">
         <v>127</v>
       </c>
       <c r="H2" s="58"/>
@@ -10282,10 +10642,10 @@
       <c r="C11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="159">
+      <c r="D11" s="154">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="E11" s="157">
+      <c r="E11" s="152">
         <f>J11*K11</f>
         <v>24969.279999999999</v>
       </c>
@@ -10392,7 +10752,7 @@
       <c r="A15" s="93">
         <v>10</v>
       </c>
-      <c r="B15" s="154" t="s">
+      <c r="B15" s="149" t="s">
         <v>189</v>
       </c>
       <c r="C15" s="32" t="s">
@@ -10462,6 +10822,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" location="'SU A0100'!A1" display="'SU A0100'!A1"/>
+    <hyperlink ref="G2" location="SU_A0100_BOM" display="Back to BOM"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10475,7 +10836,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10513,7 +10874,7 @@
       <c r="D2" s="58"/>
       <c r="E2" s="58"/>
       <c r="F2" s="58"/>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="97" t="s">
         <v>127</v>
       </c>
       <c r="H2" s="58"/>
@@ -10546,7 +10907,7 @@
       <c r="D3" s="111" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="98" t="s">
+      <c r="E3" t="s">
         <v>87</v>
       </c>
       <c r="F3" s="58"/>
@@ -10755,10 +11116,10 @@
       <c r="C11" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="159">
+      <c r="D11" s="154">
         <v>9.1999999999999998E-3</v>
       </c>
-      <c r="E11" s="157">
+      <c r="E11" s="152">
         <f>J11*K11</f>
         <v>20221.600000000002</v>
       </c>
@@ -10865,7 +11226,7 @@
       <c r="A15" s="93">
         <v>10</v>
       </c>
-      <c r="B15" s="154" t="s">
+      <c r="B15" s="149" t="s">
         <v>189</v>
       </c>
       <c r="C15" s="32" t="s">
@@ -10935,7 +11296,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" location="'SU A0100'!A1" display="'SU A0100'!A1"/>
-    <hyperlink ref="E3" location="dBR_01001" display="Drawing"/>
+    <hyperlink ref="G2" location="SU_A0100_BOM" display="Back to BOM"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>